<commit_message>
fixed epss scring and version no. validation
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pali.surdhar/Downloads/getcvefromcpe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E381E602-C842-3B45-9367-5AC45E8BFB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F671DF1-84A8-D147-B3A3-DD4EED41B109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="7" xr2:uid="{55FAB557-CDDF-9149-83BF-CB279CF13EB4}"/>
+    <workbookView xWindow="42680" yWindow="5800" windowWidth="33600" windowHeight="20500" activeTab="7" xr2:uid="{55FAB557-CDDF-9149-83BF-CB279CF13EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="product1" sheetId="1" r:id="rId1"/>
@@ -15388,10 +15388,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E301EBAE-D1E8-1C46-A4A1-0B505F843D5B}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15400,7 +15400,7 @@
     <col min="3" max="3" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -15411,7 +15411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1005</v>
       </c>
@@ -15426,7 +15426,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>1006</v>
       </c>
@@ -15441,7 +15441,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1435</v>
       </c>
@@ -15458,22 +15458,23 @@
         <v>652</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>1009</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="14" t="s">
-        <v>402</v>
-      </c>
+      <c r="C5" s="14"/>
       <c r="D5" s="4" t="s">
         <v>579</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1010</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>1132</v>
       </c>
@@ -15488,7 +15489,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>1133</v>
       </c>
@@ -15503,7 +15504,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>1134</v>
       </c>
@@ -15518,7 +15519,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>1135</v>
       </c>
@@ -15533,7 +15534,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>1136</v>
       </c>
@@ -15548,7 +15549,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>386</v>
       </c>
@@ -15563,7 +15564,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>1140</v>
       </c>
@@ -15578,7 +15579,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>1141</v>
       </c>
@@ -15593,7 +15594,7 @@
         <v>1144</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>1145</v>
       </c>
@@ -15608,7 +15609,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>1148</v>
       </c>
@@ -15623,7 +15624,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>324</v>
       </c>
@@ -15638,7 +15639,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>1154</v>
       </c>
@@ -15653,7 +15654,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>1155</v>
       </c>
@@ -15668,7 +15669,7 @@
         <v>1153</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>1</v>
       </c>
@@ -15683,7 +15684,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>1158</v>
       </c>
@@ -15698,7 +15699,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>1159</v>
       </c>
@@ -15713,7 +15714,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>1162</v>
       </c>
@@ -15728,7 +15729,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>1165</v>
       </c>
@@ -15743,7 +15744,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>1166</v>
       </c>
@@ -15758,22 +15759,23 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>1169</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="14">
-        <v>3.1</v>
-      </c>
+      <c r="C25" s="14"/>
       <c r="D25" s="4" t="s">
         <v>618</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>1170</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="I25">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>1171</v>
       </c>
@@ -15788,7 +15790,7 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>1174</v>
       </c>
@@ -15803,7 +15805,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>1176</v>
       </c>
@@ -15818,7 +15820,7 @@
         <v>1175</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>259</v>
       </c>
@@ -15833,7 +15835,7 @@
         <v>1177</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>419</v>
       </c>
@@ -15848,7 +15850,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>1180</v>
       </c>
@@ -15863,7 +15865,7 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>1183</v>
       </c>

</xml_diff>

<commit_message>
fixed version string issue
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pali.surdhar/Downloads/getcvefromcpe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F671DF1-84A8-D147-B3A3-DD4EED41B109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{607C952D-6E89-804C-B855-4B18F0E87C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42680" yWindow="5800" windowWidth="33600" windowHeight="20500" activeTab="7" xr2:uid="{55FAB557-CDDF-9149-83BF-CB279CF13EB4}"/>
+    <workbookView xWindow="3120" yWindow="7840" windowWidth="33600" windowHeight="20500" xr2:uid="{55FAB557-CDDF-9149-83BF-CB279CF13EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="product1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="1436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2629" uniqueCount="1437">
   <si>
     <t>Version</t>
   </si>
@@ -4350,6 +4350,9 @@
   </si>
   <si>
     <t>gcc</t>
+  </si>
+  <si>
+    <t>1.1.1t</t>
   </si>
 </sst>
 </file>
@@ -4868,8 +4871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D476AB9-6CD0-1D49-A45B-44D60F3B753C}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4912,7 +4915,7 @@
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="13" t="s">
-        <v>4</v>
+        <v>1436</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -5214,8 +5217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391C29E5-4BBA-BF46-82BF-4343E6666CD4}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8629,7 +8632,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8996,7 +8999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA9A4D1-C8ED-D84A-96B5-71273E61F1C3}">
   <dimension ref="A1:E400"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
+    <sheetView topLeftCell="A183" workbookViewId="0">
       <selection activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
@@ -15390,8 +15393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E301EBAE-D1E8-1C46-A4A1-0B505F843D5B}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15463,7 +15466,9 @@
         <v>1009</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="14"/>
+      <c r="C5" s="14" t="s">
+        <v>402</v>
+      </c>
       <c r="D5" s="4" t="s">
         <v>579</v>
       </c>
@@ -15764,7 +15769,9 @@
         <v>1169</v>
       </c>
       <c r="B25" s="4"/>
-      <c r="C25" s="14"/>
+      <c r="C25" s="14">
+        <v>3.1</v>
+      </c>
       <c r="D25" s="4" t="s">
         <v>618</v>
       </c>

</xml_diff>

<commit_message>
buildroot package files support
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pali.surdhar/Downloads/getcvefromcpe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECA2CFD-88BB-3C46-BB94-2DC1B3512B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E30FF6A-1108-BF44-BE13-9D6551E15532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="9" xr2:uid="{55FAB557-CDDF-9149-83BF-CB279CF13EB4}"/>
+    <workbookView xWindow="220" yWindow="1260" windowWidth="28800" windowHeight="17500" activeTab="8" xr2:uid="{55FAB557-CDDF-9149-83BF-CB279CF13EB4}"/>
   </bookViews>
   <sheets>
     <sheet name="product1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2665" uniqueCount="1444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2706" uniqueCount="1463">
   <si>
     <t>Version</t>
   </si>
@@ -4376,6 +4376,63 @@
   </si>
   <si>
     <t>update</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>pyyaml</t>
+  </si>
+  <si>
+    <t>certifi_project</t>
+  </si>
+  <si>
+    <t>2017.11.5</t>
+  </si>
+  <si>
+    <t>pypa</t>
+  </si>
+  <si>
+    <t>pip</t>
+  </si>
+  <si>
+    <t>19.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pip </t>
+  </si>
+  <si>
+    <t>setuptools</t>
+  </si>
+  <si>
+    <t>1.25.4</t>
+  </si>
+  <si>
+    <t>wheel-project</t>
+  </si>
+  <si>
+    <t>0.38.1</t>
+  </si>
+  <si>
+    <t>golang</t>
+  </si>
+  <si>
+    <t>ssh</t>
+  </si>
+  <si>
+    <t>65.5.0</t>
+  </si>
+  <si>
+    <t>0.0.0-20201203163018-be400aefbc4c</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -4495,7 +4552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4541,11 +4598,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4635,13 +4698,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4683,13 +4746,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4731,13 +4794,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4779,13 +4842,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4827,13 +4890,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4875,13 +4938,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4923,13 +4986,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -4971,13 +5034,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5019,13 +5082,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5067,13 +5130,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5115,13 +5178,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5163,13 +5226,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5211,13 +5274,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5259,13 +5322,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5307,13 +5370,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5355,13 +5418,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5403,13 +5466,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5451,13 +5514,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5499,13 +5562,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5547,13 +5610,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -5595,13 +5658,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
@@ -6307,80 +6370,164 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C798EB2C-8B4D-9545-B46F-35C870162C80}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="33.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="5" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B1" t="s">
         <v>1439</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1436</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>1438</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="20" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="F2" s="25" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>1437</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="C3" s="20" t="s">
         <v>1435</v>
       </c>
-      <c r="C3" s="20">
+      <c r="D3" s="20">
         <v>2020.01</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>1440</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20">
+      <c r="C4" s="20"/>
+      <c r="D4" s="20">
         <v>8.1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>1441</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>560</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20" t="s">
         <v>267</v>
       </c>
     </row>
+    <row r="6" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D6" s="19">
+        <v>2020.01</v>
+      </c>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>1442</v>
+      </c>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>537</v>
+      </c>
+      <c r="D8" s="19">
+        <v>8.1</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1" xr:uid="{7F308A44-950A-6947-A24B-E99FFFA2BA61}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6846,28 +6993,28 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="22" t="s">
         <v>186</v>
       </c>
       <c r="B29" s="4"/>
-      <c r="C29" s="22" t="s">
+      <c r="C29" s="23" t="s">
         <v>187</v>
       </c>
       <c r="D29" s="14"/>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="24" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4"/>
-      <c r="C30" s="22"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="14"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
@@ -17213,7 +17360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E301EBAE-D1E8-1C46-A4A1-0B505F843D5B}">
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -18682,84 +18829,150 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE13542-0EC4-264E-B120-4F2C113814E9}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1436</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>1438</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>1437</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>1435</v>
-      </c>
-      <c r="C3" s="20">
-        <v>2020.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>1442</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>537</v>
-      </c>
-      <c r="C5" s="14">
-        <v>8.1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>1441</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="F5" s="1"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>1447</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D2">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>1448</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>1449</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>1450</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>1454</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>1460</v>
+      </c>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>1457</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E9" s="21"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E5" r:id="rId1" xr:uid="{7F308A44-950A-6947-A24B-E99FFFA2BA61}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>